<commit_message>
Fine tune temperature func etc
</commit_message>
<xml_diff>
--- a/Real2020Entry1/forBot_StudentRequestsMatrix.xlsx
+++ b/Real2020Entry1/forBot_StudentRequestsMatrix.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Jun Allard</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Steven Allison</t>
   </si>
   <si>
+    <t>Kavita Arora</t>
+  </si>
+  <si>
     <t>Scott Atwood</t>
   </si>
   <si>
@@ -34,6 +37,9 @@
     <t>James Brody</t>
   </si>
   <si>
+    <t>Anne Calof</t>
+  </si>
+  <si>
     <t>Tim Downing</t>
   </si>
   <si>
@@ -79,6 +85,9 @@
     <t>Qing Nie</t>
   </si>
   <si>
+    <t>Medha Pathak</t>
+  </si>
+  <si>
     <t>Eric Potma</t>
   </si>
   <si>
@@ -100,12 +109,18 @@
     <t>Vivek Swarup</t>
   </si>
   <si>
+    <t>Kevin Thornton</t>
+  </si>
+  <si>
     <t>Alejandra Verdugo</t>
   </si>
   <si>
     <t>Armando Villalta</t>
   </si>
   <si>
+    <t>Marian Waterman</t>
+  </si>
+  <si>
     <t>Katrine Whiteson</t>
   </si>
   <si>
@@ -119,6 +134,9 @@
   </si>
   <si>
     <t>Kyoko Yokomori</t>
+  </si>
+  <si>
+    <t>Clare Yu</t>
   </si>
   <si>
     <t>Jin Yu</t>
@@ -560,15 +578,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK27"/>
+  <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -678,10 +696,28 @@
       <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:43">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -693,10 +729,10 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -791,10 +827,28 @@
       <c r="AK2">
         <v>0</v>
       </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>1</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:43">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -818,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -842,25 +896,25 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
         <v>0</v>
       </c>
       <c r="U3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3">
         <v>0</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X3">
         <v>0</v>
@@ -890,10 +944,10 @@
         <v>0</v>
       </c>
       <c r="AG3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI3">
         <v>0</v>
@@ -904,10 +958,28 @@
       <c r="AK3">
         <v>0</v>
       </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AM3">
+        <v>1</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:43">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -979,7 +1051,7 @@
         <v>0</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z4">
         <v>0</v>
@@ -1017,10 +1089,28 @@
       <c r="AK4">
         <v>0</v>
       </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:43">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1047,16 +1137,16 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1077,13 +1167,13 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5">
         <v>0</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5">
         <v>0</v>
@@ -1130,10 +1220,28 @@
       <c r="AK5">
         <v>0</v>
       </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:43">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1145,10 +1253,10 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1181,13 +1289,13 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -1243,10 +1351,28 @@
       <c r="AK6">
         <v>0</v>
       </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:43">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1356,10 +1482,28 @@
       <c r="AK7">
         <v>0</v>
       </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:43">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1371,10 +1515,10 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1398,13 +1542,13 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8">
         <v>0</v>
@@ -1419,13 +1563,13 @@
         <v>0</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8">
         <v>0</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8">
         <v>0</v>
@@ -1469,10 +1613,28 @@
       <c r="AK8">
         <v>0</v>
       </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:43">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1481,10 +1643,10 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1514,13 +1676,13 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -1532,13 +1694,13 @@
         <v>0</v>
       </c>
       <c r="U9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9">
         <v>0</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9">
         <v>0</v>
@@ -1577,15 +1739,33 @@
         <v>0</v>
       </c>
       <c r="AJ9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK9">
         <v>0</v>
       </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:43">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1615,13 +1795,13 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1681,10 +1861,10 @@
         <v>0</v>
       </c>
       <c r="AG10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI10">
         <v>0</v>
@@ -1695,10 +1875,28 @@
       <c r="AK10">
         <v>0</v>
       </c>
+      <c r="AL10">
+        <v>1</v>
+      </c>
+      <c r="AM10">
+        <v>1</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>0</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:43">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1743,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -1776,7 +1974,7 @@
         <v>0</v>
       </c>
       <c r="AA11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB11">
         <v>0</v>
@@ -1785,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="AD11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE11">
         <v>0</v>
@@ -1808,10 +2006,28 @@
       <c r="AK11">
         <v>0</v>
       </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:43">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1850,13 +2066,13 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -1883,7 +2099,7 @@
         <v>0</v>
       </c>
       <c r="Y12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z12">
         <v>0</v>
@@ -1892,7 +2108,7 @@
         <v>0</v>
       </c>
       <c r="AB12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC12">
         <v>0</v>
@@ -1910,7 +2126,7 @@
         <v>0</v>
       </c>
       <c r="AH12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI12">
         <v>0</v>
@@ -1921,10 +2137,28 @@
       <c r="AK12">
         <v>0</v>
       </c>
+      <c r="AL12">
+        <v>0</v>
+      </c>
+      <c r="AM12">
+        <v>1</v>
+      </c>
+      <c r="AN12">
+        <v>0</v>
+      </c>
+      <c r="AO12">
+        <v>0</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+      <c r="AQ12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:43">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1933,7 +2167,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1951,7 +2185,7 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1963,13 +2197,13 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -1987,16 +2221,16 @@
         <v>0</v>
       </c>
       <c r="V13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W13">
         <v>0</v>
       </c>
       <c r="X13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z13">
         <v>0</v>
@@ -2005,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="AB13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC13">
         <v>0</v>
@@ -2023,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="AH13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI13">
         <v>0</v>
@@ -2034,10 +2268,28 @@
       <c r="AK13">
         <v>0</v>
       </c>
+      <c r="AL13">
+        <v>0</v>
+      </c>
+      <c r="AM13">
+        <v>1</v>
+      </c>
+      <c r="AN13">
+        <v>0</v>
+      </c>
+      <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>0</v>
+      </c>
+      <c r="AQ13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:43">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2121,7 +2373,7 @@
         <v>0</v>
       </c>
       <c r="AC14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -2130,7 +2382,7 @@
         <v>0</v>
       </c>
       <c r="AF14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG14">
         <v>0</v>
@@ -2139,7 +2391,7 @@
         <v>0</v>
       </c>
       <c r="AI14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ14">
         <v>0</v>
@@ -2147,10 +2399,28 @@
       <c r="AK14">
         <v>0</v>
       </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <v>0</v>
+      </c>
+      <c r="AN14">
+        <v>1</v>
+      </c>
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>0</v>
+      </c>
+      <c r="AQ14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:43">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2183,13 +2453,13 @@
         <v>0</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -2198,22 +2468,22 @@
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15">
         <v>0</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15">
         <v>0</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15">
         <v>0</v>
@@ -2222,13 +2492,13 @@
         <v>0</v>
       </c>
       <c r="Y15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z15">
         <v>0</v>
       </c>
       <c r="AA15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB15">
         <v>0</v>
@@ -2237,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="AD15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE15">
         <v>0</v>
@@ -2260,10 +2530,28 @@
       <c r="AK15">
         <v>0</v>
       </c>
+      <c r="AL15">
+        <v>0</v>
+      </c>
+      <c r="AM15">
+        <v>0</v>
+      </c>
+      <c r="AN15">
+        <v>0</v>
+      </c>
+      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>0</v>
+      </c>
+      <c r="AQ15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:43">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2272,10 +2560,10 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -2302,13 +2590,13 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -2326,13 +2614,13 @@
         <v>0</v>
       </c>
       <c r="V16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W16">
         <v>0</v>
       </c>
       <c r="X16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y16">
         <v>0</v>
@@ -2373,10 +2661,28 @@
       <c r="AK16">
         <v>0</v>
       </c>
+      <c r="AL16">
+        <v>0</v>
+      </c>
+      <c r="AM16">
+        <v>0</v>
+      </c>
+      <c r="AN16">
+        <v>0</v>
+      </c>
+      <c r="AO16">
+        <v>0</v>
+      </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
+      <c r="AQ16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:43">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2436,13 +2742,13 @@
         <v>0</v>
       </c>
       <c r="U17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17">
         <v>0</v>
       </c>
       <c r="W17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X17">
         <v>0</v>
@@ -2472,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="AG17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH17">
         <v>0</v>
@@ -2486,10 +2792,28 @@
       <c r="AK17">
         <v>0</v>
       </c>
+      <c r="AL17">
+        <v>0</v>
+      </c>
+      <c r="AM17">
+        <v>0</v>
+      </c>
+      <c r="AN17">
+        <v>0</v>
+      </c>
+      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>0</v>
+      </c>
+      <c r="AQ17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:43">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -2537,25 +2861,25 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18">
         <v>0</v>
       </c>
       <c r="S18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18">
         <v>0</v>
       </c>
       <c r="U18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V18">
         <v>0</v>
       </c>
       <c r="W18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X18">
         <v>0</v>
@@ -2599,10 +2923,28 @@
       <c r="AK18">
         <v>0</v>
       </c>
+      <c r="AL18">
+        <v>0</v>
+      </c>
+      <c r="AM18">
+        <v>0</v>
+      </c>
+      <c r="AN18">
+        <v>0</v>
+      </c>
+      <c r="AO18">
+        <v>0</v>
+      </c>
+      <c r="AP18">
+        <v>0</v>
+      </c>
+      <c r="AQ18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:43">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -2641,25 +2983,25 @@
         <v>0</v>
       </c>
       <c r="N19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19">
         <v>1</v>
       </c>
       <c r="R19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19">
         <v>0</v>
@@ -2698,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="AG19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH19">
         <v>0</v>
@@ -2712,10 +3054,28 @@
       <c r="AK19">
         <v>0</v>
       </c>
+      <c r="AL19">
+        <v>1</v>
+      </c>
+      <c r="AM19">
+        <v>0</v>
+      </c>
+      <c r="AN19">
+        <v>0</v>
+      </c>
+      <c r="AO19">
+        <v>0</v>
+      </c>
+      <c r="AP19">
+        <v>0</v>
+      </c>
+      <c r="AQ19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:43">
       <c r="A20" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2748,13 +3108,13 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -2763,16 +3123,16 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20">
         <v>0</v>
@@ -2793,7 +3153,7 @@
         <v>0</v>
       </c>
       <c r="AA20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB20">
         <v>0</v>
@@ -2802,7 +3162,7 @@
         <v>0</v>
       </c>
       <c r="AD20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE20">
         <v>0</v>
@@ -2825,10 +3185,28 @@
       <c r="AK20">
         <v>0</v>
       </c>
+      <c r="AL20">
+        <v>0</v>
+      </c>
+      <c r="AM20">
+        <v>0</v>
+      </c>
+      <c r="AN20">
+        <v>0</v>
+      </c>
+      <c r="AO20">
+        <v>0</v>
+      </c>
+      <c r="AP20">
+        <v>1</v>
+      </c>
+      <c r="AQ20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:43">
       <c r="A21" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -2867,13 +3245,13 @@
         <v>0</v>
       </c>
       <c r="N21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
       <c r="P21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -2936,12 +3314,30 @@
         <v>0</v>
       </c>
       <c r="AK21">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AL21">
+        <v>0</v>
+      </c>
+      <c r="AM21">
+        <v>0</v>
+      </c>
+      <c r="AN21">
+        <v>0</v>
+      </c>
+      <c r="AO21">
+        <v>0</v>
+      </c>
+      <c r="AP21">
+        <v>1</v>
+      </c>
+      <c r="AQ21">
+        <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:43">
       <c r="A22" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2971,13 +3367,13 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -2992,13 +3388,13 @@
         <v>0</v>
       </c>
       <c r="R22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S22">
         <v>0</v>
       </c>
       <c r="T22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U22">
         <v>0</v>
@@ -3037,7 +3433,7 @@
         <v>0</v>
       </c>
       <c r="AG22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH22">
         <v>0</v>
@@ -3051,10 +3447,28 @@
       <c r="AK22">
         <v>0</v>
       </c>
+      <c r="AL22">
+        <v>1</v>
+      </c>
+      <c r="AM22">
+        <v>0</v>
+      </c>
+      <c r="AN22">
+        <v>0</v>
+      </c>
+      <c r="AO22">
+        <v>0</v>
+      </c>
+      <c r="AP22">
+        <v>0</v>
+      </c>
+      <c r="AQ22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:43">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -3090,13 +3504,13 @@
         <v>0</v>
       </c>
       <c r="M23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23">
         <v>0</v>
       </c>
       <c r="O23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P23">
         <v>0</v>
@@ -3117,13 +3531,13 @@
         <v>0</v>
       </c>
       <c r="V23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W23">
         <v>0</v>
       </c>
       <c r="X23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y23">
         <v>0</v>
@@ -3164,10 +3578,28 @@
       <c r="AK23">
         <v>0</v>
       </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="AM23">
+        <v>0</v>
+      </c>
+      <c r="AN23">
+        <v>0</v>
+      </c>
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>0</v>
+      </c>
+      <c r="AQ23">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:43">
       <c r="A24" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3218,25 +3650,25 @@
         <v>0</v>
       </c>
       <c r="R24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S24">
         <v>0</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U24">
         <v>0</v>
       </c>
       <c r="V24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W24">
         <v>0</v>
       </c>
       <c r="X24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y24">
         <v>0</v>
@@ -3263,7 +3695,7 @@
         <v>0</v>
       </c>
       <c r="AG24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH24">
         <v>0</v>
@@ -3277,10 +3709,28 @@
       <c r="AK24">
         <v>0</v>
       </c>
+      <c r="AL24">
+        <v>1</v>
+      </c>
+      <c r="AM24">
+        <v>0</v>
+      </c>
+      <c r="AN24">
+        <v>0</v>
+      </c>
+      <c r="AO24">
+        <v>0</v>
+      </c>
+      <c r="AP24">
+        <v>0</v>
+      </c>
+      <c r="AQ24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:43">
       <c r="A25" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -3390,10 +3840,28 @@
       <c r="AK25">
         <v>0</v>
       </c>
+      <c r="AL25">
+        <v>0</v>
+      </c>
+      <c r="AM25">
+        <v>0</v>
+      </c>
+      <c r="AN25">
+        <v>0</v>
+      </c>
+      <c r="AO25">
+        <v>0</v>
+      </c>
+      <c r="AP25">
+        <v>0</v>
+      </c>
+      <c r="AQ25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:43">
       <c r="A26" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -3438,13 +3906,13 @@
         <v>0</v>
       </c>
       <c r="P26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q26">
         <v>0</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26">
         <v>0</v>
@@ -3471,7 +3939,7 @@
         <v>0</v>
       </c>
       <c r="AA26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB26">
         <v>0</v>
@@ -3480,13 +3948,13 @@
         <v>0</v>
       </c>
       <c r="AD26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE26">
         <v>0</v>
       </c>
       <c r="AF26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG26">
         <v>0</v>
@@ -3501,12 +3969,30 @@
         <v>0</v>
       </c>
       <c r="AK26">
+        <v>1</v>
+      </c>
+      <c r="AL26">
+        <v>0</v>
+      </c>
+      <c r="AM26">
+        <v>0</v>
+      </c>
+      <c r="AN26">
+        <v>0</v>
+      </c>
+      <c r="AO26">
+        <v>0</v>
+      </c>
+      <c r="AP26">
+        <v>0</v>
+      </c>
+      <c r="AQ26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:43">
       <c r="A27" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -3569,13 +4055,13 @@
         <v>0</v>
       </c>
       <c r="V27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W27">
         <v>0</v>
       </c>
       <c r="X27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y27">
         <v>0</v>
@@ -3614,6 +4100,24 @@
         <v>0</v>
       </c>
       <c r="AK27">
+        <v>0</v>
+      </c>
+      <c r="AL27">
+        <v>0</v>
+      </c>
+      <c r="AM27">
+        <v>0</v>
+      </c>
+      <c r="AN27">
+        <v>0</v>
+      </c>
+      <c r="AO27">
+        <v>0</v>
+      </c>
+      <c r="AP27">
+        <v>0</v>
+      </c>
+      <c r="AQ27">
         <v>0</v>
       </c>
     </row>

</xml_diff>